<commit_message>
9th and 10th Semester Added With Other Semester Minor Changes
</commit_message>
<xml_diff>
--- a/Grade.xlsx
+++ b/Grade.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\New folder\My_University_Life\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7999558-1AA6-4DEE-9293-A8861AD78158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBA88E5-9660-4FA3-81B3-54C1F9EAF5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -681,7 +681,7 @@
   <dimension ref="B3:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -705,9 +705,7 @@
       <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="8">
-        <v>3</v>
-      </c>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="2:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
@@ -716,9 +714,7 @@
       <c r="C6" s="2">
         <v>0</v>
       </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="2:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -727,9 +723,7 @@
       <c r="C7" s="2">
         <v>10</v>
       </c>
-      <c r="D7" s="8">
-        <v>5</v>
-      </c>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="2:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -738,9 +732,7 @@
       <c r="C8" s="2">
         <v>25</v>
       </c>
-      <c r="D8" s="8">
-        <v>22</v>
-      </c>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="2:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
@@ -749,9 +741,7 @@
       <c r="C9" s="2">
         <v>30</v>
       </c>
-      <c r="D9" s="8">
-        <v>18</v>
-      </c>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="2:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
@@ -760,9 +750,7 @@
       <c r="C10" s="2">
         <v>30</v>
       </c>
-      <c r="D10" s="8">
-        <v>25</v>
-      </c>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="2:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
@@ -774,7 +762,7 @@
       </c>
       <c r="D11" s="10">
         <f>SUM(D5:D10)</f>
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,7 +772,7 @@
       </c>
       <c r="D12" s="23" t="str">
         <f>VLOOKUP(D11,Sheet2!$C$3:$D$12,2)</f>
-        <v>A-</v>
+        <v>F</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -794,7 +782,7 @@
       </c>
       <c r="D13" s="12">
         <f>VLOOKUP(D12,Sheet2!$D$3:$E$12,2,FALSE)</f>
-        <v>3.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>